<commit_message>
jmxor's design is started
</commit_message>
<xml_diff>
--- a/instrucitons.xlsx
+++ b/instrucitons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\University\DataPath---CSE-3038-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFF626-140C-465C-8131-44B50AF9F847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C968A20B-6781-40CD-8750-2BA1262D7D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
   <dimension ref="A4:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
zero extend added into the system
</commit_message>
<xml_diff>
--- a/instrucitons.xlsx
+++ b/instrucitons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\University\DataPath---CSE-3038-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CFE276-1088-4AAE-BDAE-82333212784F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC4456F-E378-4B3C-9B42-E8180072F484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
+    <workbookView xWindow="1380" yWindow="1950" windowWidth="21600" windowHeight="13380" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="99">
   <si>
     <t>brv</t>
   </si>
@@ -318,6 +318,21 @@
   </si>
   <si>
     <t>balnControl</t>
+  </si>
+  <si>
+    <t>brvControl</t>
+  </si>
+  <si>
+    <t>jmxorControl</t>
+  </si>
+  <si>
+    <t>branch if v=1</t>
+  </si>
+  <si>
+    <t>xor and jump</t>
+  </si>
+  <si>
+    <t>100001</t>
   </si>
 </sst>
 </file>
@@ -538,6 +553,18 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,18 +584,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -905,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8558FA9-F41A-4C66-A0E1-9ACDDCC3A203}">
-  <dimension ref="A4:Y28"/>
+  <dimension ref="A4:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +940,9 @@
     <col min="13" max="13" width="14.42578125" style="2" customWidth="1"/>
     <col min="14" max="14" width="32.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1310,11 +1327,11 @@
       <c r="E10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
       <c r="J10" s="17" t="s">
         <v>34</v>
       </c>
@@ -1375,11 +1392,11 @@
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
       <c r="J11" s="17" t="s">
         <v>34</v>
       </c>
@@ -1440,11 +1457,11 @@
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
       <c r="J12" s="17" t="s">
         <v>34</v>
       </c>
@@ -1478,11 +1495,11 @@
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
       <c r="J13" s="17" t="s">
         <v>34</v>
       </c>
@@ -1532,13 +1549,13 @@
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
       <c r="J15" s="21" t="s">
         <v>34</v>
       </c>
@@ -1566,13 +1583,13 @@
       <c r="C16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
       <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1609,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1601,14 +1618,18 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1617,303 +1638,426 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="14" t="s">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G25" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H25" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K25" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="L19" s="35" t="s">
+      <c r="L25" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="M19" s="35" t="s">
+      <c r="M25" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="N19" s="35" t="s">
+      <c r="N25" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="36" t="s">
+      <c r="O25" s="28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="6" t="s">
+      <c r="P25" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q25" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="L20" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="C26" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="9"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="L21" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="C27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="9"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="C28" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="C29" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="L29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="9"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="L24" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="9"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K30" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="L30" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="N25" s="32"/>
-      <c r="O25" s="9"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="33" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="9"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="O26" s="9"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="9"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="9"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="O34" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q34" s="9"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="P35" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q35" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
design and implement  done (??)
</commit_message>
<xml_diff>
--- a/instrucitons.xlsx
+++ b/instrucitons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\University\DataPath---CSE-3038-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E02C831-8FBF-4D4F-BF0B-2E8CECF95F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CC4DDD-3A45-43D6-8C68-EE591089400C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1920" windowWidth="21600" windowHeight="12480" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51791857-30F8-4E61-A5BF-5EA7055FA251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -611,9 +611,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -952,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8558FA9-F41A-4C66-A0E1-9ACDDCC3A203}">
   <dimension ref="A4:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +1927,7 @@
       <c r="I29" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="J29" s="39" t="s">
+      <c r="J29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K29" s="1" t="s">
@@ -2039,10 +2036,10 @@
       <c r="J31" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="K31" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="L31" s="39" t="s">
+      <c r="K31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>67</v>
       </c>
       <c r="M31" s="1" t="s">

</xml_diff>